<commit_message>
processing loop state machines started (Gerüst steht)
</commit_message>
<xml_diff>
--- a/LoggerFSM.xlsx
+++ b/LoggerFSM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="0" windowWidth="23260" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="11740" yWindow="0" windowWidth="23260" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Logger" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="131">
   <si>
     <t>check if sensor's config is in file</t>
   </si>
@@ -344,6 +344,75 @@
   </si>
   <si>
     <t>setFilterToAddressed</t>
+  </si>
+  <si>
+    <t>S_S_Started,</t>
+  </si>
+  <si>
+    <t>S_S_InitializedCANBus</t>
+  </si>
+  <si>
+    <t>S_S_RetrievedSerialNumber</t>
+  </si>
+  <si>
+    <t>S_S_CommThreadListeningForBroadcastMessages</t>
+  </si>
+  <si>
+    <t>S_S_SerialNumberSent</t>
+  </si>
+  <si>
+    <t>S_S_CANIDReceived</t>
+  </si>
+  <si>
+    <t>S_S_ConfigurationReceived</t>
+  </si>
+  <si>
+    <t>S_S_TimeSyncReceived</t>
+  </si>
+  <si>
+    <t>S_S_OperationLoopStarted</t>
+  </si>
+  <si>
+    <t>S_S_RecordingRawData</t>
+  </si>
+  <si>
+    <t>S_S_DetectingEvents</t>
+  </si>
+  <si>
+    <t>S_S_NotRecording</t>
+  </si>
+  <si>
+    <t>S_L_Started</t>
+  </si>
+  <si>
+    <t>S_L_SDCardDetected</t>
+  </si>
+  <si>
+    <t>S_L_ConfigurationReady</t>
+  </si>
+  <si>
+    <t>S_L_WaitForSerialNumbers</t>
+  </si>
+  <si>
+    <t>S_L_SendOutConfigurations</t>
+  </si>
+  <si>
+    <t>S_L_SendOutTimeSyncs</t>
+  </si>
+  <si>
+    <t>S_L_AllSensorsReady</t>
+  </si>
+  <si>
+    <t>S_L_ProcessingHoldingToken</t>
+  </si>
+  <si>
+    <t>S_L_ProcessingWaitingForData</t>
+  </si>
+  <si>
+    <t>Sensor Unit States</t>
+  </si>
+  <si>
+    <t>Logger States:</t>
   </si>
 </sst>
 </file>
@@ -407,8 +476,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -507,7 +610,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -553,6 +656,23 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -598,6 +718,23 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -934,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1240,205 +1377,279 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>64</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>65</v>
       </c>
       <c r="E32" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7">
       <c r="A33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>70</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>69</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7">
       <c r="A35" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="4"/>
-      <c r="B36" t="s">
+    <row r="36" spans="1:7">
+      <c r="A36" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
         <v>71</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:7">
       <c r="A37" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>72</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>73</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="4"/>
+    <row r="39" spans="1:7">
+      <c r="A39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="4"/>
       <c r="E39" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="4"/>
-      <c r="B40" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:7">
       <c r="A43" s="4"/>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:7">
       <c r="A44" s="4"/>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:7">
       <c r="A45" s="4"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:7">
       <c r="A46" s="4"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:7">
       <c r="A47" s="4"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:7">
       <c r="A48" s="4"/>
       <c r="E48" s="4"/>
     </row>

</xml_diff>